<commit_message>
Added missing PartialBatch measurement results for scale 1,2,4 #28
</commit_message>
<xml_diff>
--- a/tests/org.eclipse.incquery.examples.cps.performance.tests/results/StatisticsBased_ToolchainPerf_Scale_1_2_4.xlsx
+++ b/tests/org.eclipse.incquery.examples.cps.performance.tests/results/StatisticsBased_ToolchainPerf_Scale_1_2_4.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="35">
   <si>
     <t>BatchSimple</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>SUMeReferences</t>
+  </si>
+  <si>
+    <t>PartialBatch</t>
   </si>
 </sst>
 </file>
@@ -797,6 +800,64 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>memory!$J$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PartialBatch Distributed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>memory!$F$38:$F$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>133228</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>114373</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>135403</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -807,11 +868,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1186008768"/>
-        <c:axId val="1186009312"/>
+        <c:axId val="-2140565200"/>
+        <c:axId val="-2140558128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1186008768"/>
+        <c:axId val="-2140565200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -854,7 +915,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1186009312"/>
+        <c:crossAx val="-2140558128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -862,7 +923,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1186009312"/>
+        <c:axId val="-2140558128"/>
         <c:scaling>
           <c:logBase val="4"/>
           <c:orientation val="minMax"/>
@@ -915,7 +976,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1186008768"/>
+        <c:crossAx val="-2140565200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1544,6 +1605,64 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>memory!$J$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PartialBatch Distributed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>memory!$G$38:$G$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>244459</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>307606</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>321331</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1554,11 +1673,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1186009856"/>
-        <c:axId val="1186000064"/>
+        <c:axId val="-2140563568"/>
+        <c:axId val="-2140561392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1186009856"/>
+        <c:axId val="-2140563568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1601,7 +1720,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1186000064"/>
+        <c:crossAx val="-2140561392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1609,7 +1728,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1186000064"/>
+        <c:axId val="-2140561392"/>
         <c:scaling>
           <c:logBase val="4"/>
           <c:orientation val="minMax"/>
@@ -1662,7 +1781,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1186009856"/>
+        <c:crossAx val="-2140563568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1788,7 +1907,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1864,7 +1982,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>time!$B$2:$B$4</c:f>
+              <c:f>time!$B$38:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1940,7 +2058,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>time!$B$2:$B$4</c:f>
+              <c:f>time!$B$38:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2016,7 +2134,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>time!$B$2:$B$4</c:f>
+              <c:f>time!$B$38:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2098,7 +2216,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>time!$B$2:$B$4</c:f>
+              <c:f>time!$B$38:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2180,7 +2298,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>time!$B$2:$B$4</c:f>
+              <c:f>time!$B$38:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2256,7 +2374,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>time!$B$2:$B$4</c:f>
+              <c:f>time!$B$38:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2286,6 +2404,82 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4525</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>time!$M$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PartialBatch Distributed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>time!$B$38:$B$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>time!$G$38:$G$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2280</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2087</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2302,11 +2496,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="738120176"/>
-        <c:axId val="738113104"/>
+        <c:axId val="-185073792"/>
+        <c:axId val="-185065088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="738120176"/>
+        <c:axId val="-185073792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2349,7 +2543,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="738113104"/>
+        <c:crossAx val="-185065088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2357,7 +2551,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="738113104"/>
+        <c:axId val="-185065088"/>
         <c:scaling>
           <c:logBase val="4"/>
           <c:orientation val="minMax"/>
@@ -2410,7 +2604,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="738120176"/>
+        <c:crossAx val="-185073792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2424,7 +2618,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2536,7 +2729,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3040,6 +3232,64 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>time!$M$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PartialBatch Distributed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>time!$I$38:$I$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -3050,11 +3300,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1046236736"/>
-        <c:axId val="1046224768"/>
+        <c:axId val="-185071616"/>
+        <c:axId val="-185068352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1046236736"/>
+        <c:axId val="-185071616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3097,7 +3347,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1046224768"/>
+        <c:crossAx val="-185068352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3105,7 +3355,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1046224768"/>
+        <c:axId val="-185068352"/>
         <c:scaling>
           <c:logBase val="4"/>
           <c:orientation val="minMax"/>
@@ -3157,7 +3407,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1046236736"/>
+        <c:crossAx val="-185071616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3171,7 +3421,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3283,7 +3532,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3359,7 +3607,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>time!$B$2:$B$4</c:f>
+              <c:f>time!$B$38:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3435,7 +3683,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>time!$B$2:$B$4</c:f>
+              <c:f>time!$B$38:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3511,7 +3759,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>time!$B$2:$B$4</c:f>
+              <c:f>time!$B$38:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3593,7 +3841,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>time!$B$2:$B$4</c:f>
+              <c:f>time!$B$38:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3675,7 +3923,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>time!$B$2:$B$4</c:f>
+              <c:f>time!$B$38:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3751,7 +3999,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>time!$B$2:$B$4</c:f>
+              <c:f>time!$B$38:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3781,6 +4029,82 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2472</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>time!$M$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PartialBatch Distributed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>time!$B$38:$B$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>time!$H$41:$H$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1071</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1713</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3749</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3797,11 +4121,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1210505472"/>
-        <c:axId val="1210506016"/>
+        <c:axId val="-229384704"/>
+        <c:axId val="-175456192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1210505472"/>
+        <c:axId val="-229384704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3844,7 +4168,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1210506016"/>
+        <c:crossAx val="-175456192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3852,7 +4176,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1210506016"/>
+        <c:axId val="-175456192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3903,7 +4227,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1210505472"/>
+        <c:crossAx val="-229384704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3917,7 +4241,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4025,7 +4348,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4229,11 +4551,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1210512000"/>
-        <c:axId val="1210512544"/>
+        <c:axId val="-2066823344"/>
+        <c:axId val="-2066834768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1210512000"/>
+        <c:axId val="-2066823344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4276,7 +4598,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1210512544"/>
+        <c:crossAx val="-2066834768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4284,7 +4606,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1210512544"/>
+        <c:axId val="-2066834768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4335,7 +4657,7 @@
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1210512000"/>
+        <c:crossAx val="-2066823344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4349,7 +4671,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7842,14 +8163,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>537885</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:colOff>560297</xdr:colOff>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>33618</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>8968</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:colOff>31380</xdr:colOff>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>3083</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8141,10 +8462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="X43" sqref="X43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9269,11 +9590,153 @@
         <v>ViatraTransformation JDT-based</v>
       </c>
     </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38">
+        <v>231368</v>
+      </c>
+      <c r="E38">
+        <v>124176</v>
+      </c>
+      <c r="F38">
+        <v>133228</v>
+      </c>
+      <c r="G38">
+        <v>244459</v>
+      </c>
+      <c r="H38" t="s">
+        <v>19</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" ref="J38:J43" si="1">CONCATENATE(C38," ",H38)</f>
+        <v>PartialBatch Distributed</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39">
+        <v>116348</v>
+      </c>
+      <c r="E39">
+        <v>122508</v>
+      </c>
+      <c r="F39">
+        <v>114373</v>
+      </c>
+      <c r="G39">
+        <v>307606</v>
+      </c>
+      <c r="H39" t="s">
+        <v>19</v>
+      </c>
+      <c r="J39" t="str">
+        <f t="shared" si="1"/>
+        <v>PartialBatch Distributed</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40">
+        <v>141860</v>
+      </c>
+      <c r="E40">
+        <v>133949</v>
+      </c>
+      <c r="F40">
+        <v>135403</v>
+      </c>
+      <c r="G40">
+        <v>321331</v>
+      </c>
+      <c r="H40" t="s">
+        <v>19</v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" si="1"/>
+        <v>PartialBatch Distributed</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41">
+        <v>135382</v>
+      </c>
+      <c r="E41">
+        <v>140715</v>
+      </c>
+      <c r="F41">
+        <v>130863</v>
+      </c>
+      <c r="G41">
+        <v>235643</v>
+      </c>
+      <c r="H41" t="s">
+        <v>20</v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" si="1"/>
+        <v>PartialBatch JDT-based</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42">
+        <v>128080</v>
+      </c>
+      <c r="E42">
+        <v>150704</v>
+      </c>
+      <c r="F42">
+        <v>125160</v>
+      </c>
+      <c r="G42">
+        <v>294658</v>
+      </c>
+      <c r="H42" t="s">
+        <v>20</v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" si="1"/>
+        <v>PartialBatch JDT-based</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43">
+        <v>298743</v>
+      </c>
+      <c r="E43">
+        <v>143800</v>
+      </c>
+      <c r="F43">
+        <v>147198</v>
+      </c>
+      <c r="G43">
+        <v>342142</v>
+      </c>
+      <c r="H43" t="s">
+        <v>20</v>
+      </c>
+      <c r="J43" t="str">
+        <f t="shared" si="1"/>
+        <v>PartialBatch JDT-based</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="B2:H37">
-    <sortCondition ref="C2:C37"/>
-    <sortCondition ref="H2:H37"/>
-    <sortCondition ref="B2:B37"/>
+  <sortState ref="C38:J43">
+    <sortCondition ref="H38:H43"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9284,8 +9747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView topLeftCell="E25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O52" sqref="O52"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O48" sqref="O48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10744,39 +11207,237 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38">
+        <v>253</v>
+      </c>
+      <c r="E38">
+        <v>122</v>
+      </c>
+      <c r="F38">
+        <v>175</v>
+      </c>
+      <c r="G38">
+        <v>2280</v>
+      </c>
+      <c r="H38">
+        <v>1731</v>
+      </c>
+      <c r="I38">
+        <v>104</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38" t="s">
+        <v>19</v>
+      </c>
       <c r="M38" t="str">
         <f t="shared" ref="M38:M66" si="1">CONCATENATE(C38," ",K38)</f>
-        <v xml:space="preserve"> </v>
+        <v>PartialBatch Distributed</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39">
+        <v>83</v>
+      </c>
+      <c r="E39">
+        <v>116</v>
+      </c>
+      <c r="F39">
+        <v>6</v>
+      </c>
+      <c r="G39">
+        <v>1993</v>
+      </c>
+      <c r="H39">
+        <v>2034</v>
+      </c>
+      <c r="I39">
+        <v>39</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39" t="s">
+        <v>19</v>
+      </c>
       <c r="M39" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+        <v>PartialBatch Distributed</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40">
+        <v>148</v>
+      </c>
+      <c r="E40">
+        <v>64</v>
+      </c>
+      <c r="F40">
+        <v>6</v>
+      </c>
+      <c r="G40">
+        <v>2087</v>
+      </c>
+      <c r="H40">
+        <v>3647</v>
+      </c>
+      <c r="I40">
+        <v>67</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40" t="s">
+        <v>19</v>
+      </c>
       <c r="M40" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+        <v>PartialBatch Distributed</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41">
+        <v>50</v>
+      </c>
+      <c r="E41">
+        <v>40</v>
+      </c>
+      <c r="F41">
+        <v>21</v>
+      </c>
+      <c r="G41">
+        <v>1906</v>
+      </c>
+      <c r="H41">
+        <v>1071</v>
+      </c>
+      <c r="I41">
+        <v>46</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41" t="s">
+        <v>20</v>
+      </c>
       <c r="M41" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+        <v>PartialBatch JDT-based</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42">
+        <v>50</v>
+      </c>
+      <c r="E42">
+        <v>67</v>
+      </c>
+      <c r="F42">
+        <v>5</v>
+      </c>
+      <c r="G42">
+        <v>1983</v>
+      </c>
+      <c r="H42">
+        <v>1713</v>
+      </c>
+      <c r="I42">
+        <v>45</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42" t="s">
+        <v>20</v>
+      </c>
       <c r="M42" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+        <v>PartialBatch JDT-based</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43">
+        <v>225</v>
+      </c>
+      <c r="E43">
+        <v>95</v>
+      </c>
+      <c r="F43">
+        <v>6</v>
+      </c>
+      <c r="G43">
+        <v>2240</v>
+      </c>
+      <c r="H43">
+        <v>3749</v>
+      </c>
+      <c r="I43">
+        <v>58</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43" t="s">
+        <v>20</v>
+      </c>
       <c r="M43" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> </v>
+        <v>PartialBatch JDT-based</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -10962,10 +11623,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12167,6 +12828,198 @@
         <v>20</v>
       </c>
     </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38">
+        <v>395</v>
+      </c>
+      <c r="C38">
+        <v>772</v>
+      </c>
+      <c r="D38">
+        <v>366</v>
+      </c>
+      <c r="E38">
+        <v>736</v>
+      </c>
+      <c r="F38">
+        <v>354</v>
+      </c>
+      <c r="G38">
+        <v>720</v>
+      </c>
+      <c r="H38">
+        <v>1115</v>
+      </c>
+      <c r="I38">
+        <v>2228</v>
+      </c>
+      <c r="J38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39">
+        <v>395</v>
+      </c>
+      <c r="C39">
+        <v>772</v>
+      </c>
+      <c r="D39">
+        <v>366</v>
+      </c>
+      <c r="E39">
+        <v>736</v>
+      </c>
+      <c r="F39">
+        <v>354</v>
+      </c>
+      <c r="G39">
+        <v>720</v>
+      </c>
+      <c r="H39">
+        <v>1115</v>
+      </c>
+      <c r="I39">
+        <v>2228</v>
+      </c>
+      <c r="J39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40">
+        <v>849</v>
+      </c>
+      <c r="C40">
+        <v>1821</v>
+      </c>
+      <c r="D40">
+        <v>773</v>
+      </c>
+      <c r="E40">
+        <v>1535</v>
+      </c>
+      <c r="F40">
+        <v>762</v>
+      </c>
+      <c r="G40">
+        <v>1535</v>
+      </c>
+      <c r="H40">
+        <v>2384</v>
+      </c>
+      <c r="I40">
+        <v>4891</v>
+      </c>
+      <c r="J40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41">
+        <v>849</v>
+      </c>
+      <c r="C41">
+        <v>1821</v>
+      </c>
+      <c r="D41">
+        <v>773</v>
+      </c>
+      <c r="E41">
+        <v>1536</v>
+      </c>
+      <c r="F41">
+        <v>762</v>
+      </c>
+      <c r="G41">
+        <v>1535</v>
+      </c>
+      <c r="H41">
+        <v>2384</v>
+      </c>
+      <c r="I41">
+        <v>4892</v>
+      </c>
+      <c r="J41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42">
+        <v>1694</v>
+      </c>
+      <c r="C42">
+        <v>4697</v>
+      </c>
+      <c r="D42">
+        <v>1534</v>
+      </c>
+      <c r="E42">
+        <v>2971</v>
+      </c>
+      <c r="F42">
+        <v>1522</v>
+      </c>
+      <c r="G42">
+        <v>3056</v>
+      </c>
+      <c r="H42">
+        <v>4750</v>
+      </c>
+      <c r="I42">
+        <v>10724</v>
+      </c>
+      <c r="J42" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43">
+        <v>1694</v>
+      </c>
+      <c r="C43">
+        <v>4697</v>
+      </c>
+      <c r="D43">
+        <v>1534</v>
+      </c>
+      <c r="E43">
+        <v>2973</v>
+      </c>
+      <c r="F43">
+        <v>1522</v>
+      </c>
+      <c r="G43">
+        <v>3056</v>
+      </c>
+      <c r="H43">
+        <v>4750</v>
+      </c>
+      <c r="I43">
+        <v>10726</v>
+      </c>
+      <c r="J43" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>